<commit_message>
Update 6 new business rule and delete 1 business rule of LocPhan
</commit_message>
<xml_diff>
--- a/Requirement Management/Software Requirement Specification/[PIM]Functional Requirement and Business Rule.xlsx
+++ b/Requirement Management/Software Requirement Specification/[PIM]Functional Requirement and Business Rule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="17400" windowHeight="8385" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="17400" windowHeight="8385" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Funtional Requirements" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="200">
   <si>
     <t>Description</t>
   </si>
@@ -247,10 +247,6 @@
   <si>
     <t>When HRD staff update and fix information (detail information,
  extend information, profile….) must be logged.</t>
-  </si>
-  <si>
-    <t>Assessment management do once a year, and HRD staff 
-must update information about reward.</t>
   </si>
   <si>
     <t>System log time use of facilitate and staff must have bond about 
@@ -451,17 +447,10 @@
     <t>Manage facilitate</t>
   </si>
   <si>
-    <t>Manage reward 
-&amp; manage discipline</t>
-  </si>
-  <si>
     <t>General (change)</t>
   </si>
   <si>
     <t xml:space="preserve">Create new information is not empty value </t>
-  </si>
-  <si>
-    <t>Quản lý khen thưởng và kỉ luật: xử lí thông tin 1 năm thì cập nhật vào ql đánh giá. Hỏi cần phần mềm làm sao chỗ này</t>
   </si>
   <si>
     <t>Functional concerned</t>
@@ -630,6 +619,51 @@
   </si>
   <si>
     <t>Gathering  information about work of staff, lectures, discipline, reward. And assessments will be updated in end of year. From this assessments help to count salary.</t>
+  </si>
+  <si>
+    <t>BR12</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Save follow format: dd-mm-yy</t>
+  </si>
+  <si>
+    <t>BR13</t>
+  </si>
+  <si>
+    <t>Export information</t>
+  </si>
+  <si>
+    <t>When export a file: format is excel file with a file report and format is doc file with a file notify</t>
+  </si>
+  <si>
+    <t>BR14</t>
+  </si>
+  <si>
+    <t>Progress must export by table</t>
+  </si>
+  <si>
+    <t>BR15</t>
+  </si>
+  <si>
+    <t>Format a file: Times New Roman font, 13 font size, Black font color. Capital and bold with title file. Capital with category title</t>
+  </si>
+  <si>
+    <t>BR16</t>
+  </si>
+  <si>
+    <t>When export a file, user must choose path and can review before export</t>
+  </si>
+  <si>
+    <t>BR17</t>
+  </si>
+  <si>
+    <t>Category use for whole system</t>
+  </si>
+  <si>
+    <t>BR18</t>
   </si>
 </sst>
 </file>
@@ -709,7 +743,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,12 +759,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,22 +849,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -855,6 +869,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -864,9 +893,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -876,17 +902,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,27 +1226,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1250,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>37</v>
@@ -1267,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>38</v>
@@ -1284,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>39</v>
@@ -1301,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>34</v>
@@ -1318,10 +1338,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>45</v>
@@ -1335,7 +1355,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
@@ -1352,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>40</v>
@@ -1369,13 +1389,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>27</v>
@@ -1386,10 +1406,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>48</v>
@@ -1403,12 +1423,12 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -1420,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>42</v>
@@ -1437,7 +1457,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
@@ -1454,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>36</v>
@@ -1471,16 +1491,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>146</v>
+        <v>134</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>143</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1488,16 +1508,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1505,16 +1525,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1522,27 +1542,27 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>18</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>135</v>
+      <c r="B22" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>59</v>
@@ -1556,7 +1576,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>28</v>
@@ -1573,7 +1593,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>19</v>
@@ -1597,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,29 +1633,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
@@ -1658,7 +1678,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1675,7 +1695,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1692,29 +1712,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="26" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>72</v>
@@ -1726,124 +1746,194 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>42</v>
+      <c r="B10" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
+        <v>73</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>131</v>
+        <v>74</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>23</v>
+      <c r="B14" s="35"/>
+      <c r="C14" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="27" t="s">
-        <v>132</v>
+      <c r="A15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>128</v>
+      <c r="E16" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:D3"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1869,24 +1959,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1907,13 +1997,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1921,13 +2011,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1935,13 +2025,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1949,13 +2039,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1963,13 +2053,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1977,40 +2067,40 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+        <v>87</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="33"/>
+        <v>82</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2018,21 +2108,21 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="33"/>
+        <v>82</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2040,21 +2130,21 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="33"/>
+        <v>82</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2062,21 +2152,21 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="33"/>
+        <v>82</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2084,21 +2174,21 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="33"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="27"/>
       <c r="L15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2106,185 +2196,185 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
+        <v>79</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+        <v>79</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+        <v>79</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
+        <v>79</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -2300,20 +2390,20 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2347,157 +2437,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="38" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="41" t="s">
+    <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="D6" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="40" t="s">
+      <c r="D9" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="41" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-    </row>
-    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="41" t="s">
+      <c r="D11" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="12" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>103</v>
+      <c r="A12" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>